<commit_message>
Emailing and Downloading Data Implemented
</commit_message>
<xml_diff>
--- a/myproject/media/KMC_Master_Checkin.xlsx
+++ b/myproject/media/KMC_Master_Checkin.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="166">
   <si>
     <t>barcode</t>
   </si>
@@ -332,6 +332,186 @@
   </si>
   <si>
     <t>Hemophilia A</t>
+  </si>
+  <si>
+    <t>ythompson@umich.edu</t>
+  </si>
+  <si>
+    <t>Nanotechnology 204</t>
+  </si>
+  <si>
+    <t>Dr. Taylor</t>
+  </si>
+  <si>
+    <t>Dylan Brown</t>
+  </si>
+  <si>
+    <t>Lab Assistant</t>
+  </si>
+  <si>
+    <t>Nanotechnology</t>
+  </si>
+  <si>
+    <t>University of Michigan</t>
+  </si>
+  <si>
+    <t>Material Analysis</t>
+  </si>
+  <si>
+    <t>Quantum Dots</t>
+  </si>
+  <si>
+    <t>12:02:49</t>
+  </si>
+  <si>
+    <t>2024-06-06</t>
+  </si>
+  <si>
+    <t>cjones@umich.edu</t>
+  </si>
+  <si>
+    <t>Mechanical Engineering 2B</t>
+  </si>
+  <si>
+    <t>Dr. Arnold</t>
+  </si>
+  <si>
+    <t>Ava White</t>
+  </si>
+  <si>
+    <t>Project Engineer</t>
+  </si>
+  <si>
+    <t>Machine Design</t>
+  </si>
+  <si>
+    <t>Autonomous Vehicles</t>
+  </si>
+  <si>
+    <t>swilliams@cam.ac.uk</t>
+  </si>
+  <si>
+    <t>Computer Science 220</t>
+  </si>
+  <si>
+    <t>new_instructor</t>
+  </si>
+  <si>
+    <t>Kiera Patel</t>
+  </si>
+  <si>
+    <t>Software Developer</t>
+  </si>
+  <si>
+    <t>Computer Science</t>
+  </si>
+  <si>
+    <t>University of Cambridge</t>
+  </si>
+  <si>
+    <t>Algorithm Development</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence Safety</t>
+  </si>
+  <si>
+    <t>tunderwood@uoftoronto.ca</t>
+  </si>
+  <si>
+    <t>Pharmacology 410</t>
+  </si>
+  <si>
+    <t>Dr. Martinez</t>
+  </si>
+  <si>
+    <t>Liam Wong</t>
+  </si>
+  <si>
+    <t>Clinical Trial Volunteer</t>
+  </si>
+  <si>
+    <t>Pharmacology</t>
+  </si>
+  <si>
+    <t>University of Toronto</t>
+  </si>
+  <si>
+    <t>Drug Tester</t>
+  </si>
+  <si>
+    <t>Alcoholism</t>
+  </si>
+  <si>
+    <t>bsmith@ucla.edu</t>
+  </si>
+  <si>
+    <t>Dr. Monroe</t>
+  </si>
+  <si>
+    <t>Jane Doe</t>
+  </si>
+  <si>
+    <t>Volunteer 2</t>
+  </si>
+  <si>
+    <t>Surgical Assistant</t>
+  </si>
+  <si>
+    <t>Appendicitis Surgery</t>
+  </si>
+  <si>
+    <t>12:08:34</t>
+  </si>
+  <si>
+    <t>jdoe@ucsd.edu</t>
+  </si>
+  <si>
+    <t>John Smith</t>
+  </si>
+  <si>
+    <t>Tissue Repair</t>
+  </si>
+  <si>
+    <t>Torn Ligament</t>
+  </si>
+  <si>
+    <t>djohnson@harvard.edu</t>
+  </si>
+  <si>
+    <t>Susan Lee</t>
+  </si>
+  <si>
+    <t>Wound Healing</t>
+  </si>
+  <si>
+    <t>Burn Treatment</t>
+  </si>
+  <si>
+    <t>kwilliams@mit.edu</t>
+  </si>
+  <si>
+    <t>Michael Brown</t>
+  </si>
+  <si>
+    <t>Robotic Surgery</t>
+  </si>
+  <si>
+    <t>Heart Surgery</t>
+  </si>
+  <si>
+    <t>tmartinez@stanford.edu</t>
+  </si>
+  <si>
+    <t>Lisa White</t>
+  </si>
+  <si>
+    <t>Statistical Analysis</t>
+  </si>
+  <si>
+    <t>Post-Surgery Recovery</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -402,7 +582,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -414,6 +594,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -724,25 +907,25 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21">
@@ -1196,6 +1379,453 @@
         <v>23</v>
       </c>
     </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="A12" s="3">
+        <v>633647</v>
+      </c>
+      <c r="B12" s="3">
+        <v>147312</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="A13" s="3">
+        <v>421305</v>
+      </c>
+      <c r="B13" s="3">
+        <v>134530</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="A14" s="3">
+        <v>734628</v>
+      </c>
+      <c r="B14" s="3">
+        <v>130463</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="A15" s="3">
+        <v>825739</v>
+      </c>
+      <c r="B15" s="3">
+        <v>131044</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+      <c r="A16" s="3">
+        <v>168162</v>
+      </c>
+      <c r="B16" s="3">
+        <v>126977</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+      <c r="A17" s="3">
+        <v>423517</v>
+      </c>
+      <c r="B17" s="3">
+        <v>124153</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+      <c r="A18" s="3">
+        <v>423518</v>
+      </c>
+      <c r="B18" s="3">
+        <v>124154</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+      <c r="A19" s="3">
+        <v>423519</v>
+      </c>
+      <c r="B19" s="3">
+        <v>124155</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+      <c r="A20" s="3">
+        <v>423520</v>
+      </c>
+      <c r="B20" s="3">
+        <v>124156</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+      <c r="A21" s="3">
+        <v>423521</v>
+      </c>
+      <c r="B21" s="3">
+        <v>124157</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="M22" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>